<commit_message>
VSKP EXCEL COL FORMS
</commit_message>
<xml_diff>
--- a/Dashboard/media/overall.xlsx
+++ b/Dashboard/media/overall.xlsx
@@ -1,21 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24729"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\__gitam__\DashBoard-BackEnd\Dashboard\media\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{963C48E1-5E77-4D74-A8B9-13BDA6AF7731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="9405"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="CF 2022" sheetId="1" r:id="rId1"/>
-    <sheet name="2022 Data on Other Career Optio" sheetId="2" r:id="rId2"/>
+    <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="45">
   <si>
     <t>2022 OVERALL CAREER FULFILLMENT STATISTICS - GCGC</t>
   </si>
@@ -86,9 +100,6 @@
     <t>Total No. of students in the first year of present final year batch.</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>Total No. of students in final year.</t>
   </si>
   <si>
@@ -153,55 +164,13 @@
   </si>
   <si>
     <t>(c) Average (Per annum)Rs.in lakhs</t>
-  </si>
-  <si>
-    <t>Career Option</t>
-  </si>
-  <si>
-    <t>Career Guidance Center - Visakhapatnam</t>
-  </si>
-  <si>
-    <t>Career Guidance Center - Hyderabad</t>
-  </si>
-  <si>
-    <t>Career Guidance Center - Bengaluru</t>
-  </si>
-  <si>
-    <t>SoT</t>
-  </si>
-  <si>
-    <t>Placements</t>
-  </si>
-  <si>
-    <t>Deferred Placements</t>
-  </si>
-  <si>
-    <t>Higher Education Overseas</t>
-  </si>
-  <si>
-    <t>Higher Education India</t>
-  </si>
-  <si>
-    <t>Entrepreneurship /Startups</t>
-  </si>
-  <si>
-    <t>Family Business</t>
-  </si>
-  <si>
-    <t>CIVILS/UPSC/SSC/GROUPS</t>
-  </si>
-  <si>
-    <t>Yet to Disclose</t>
-  </si>
-  <si>
-    <t>Not interested</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -212,27 +181,32 @@
       <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color rgb="FFFFFFFF"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -250,39 +224,26 @@
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Courier New"/>
+      <family val="3"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FFC00000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <color theme="1"/>
       <name val="Courier New"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="11">
@@ -510,7 +471,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -628,46 +589,27 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -683,18 +625,13 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -705,6 +642,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -907,7 +847,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
@@ -992,140 +932,140 @@
       <c r="AN1" s="1"/>
     </row>
     <row r="2" spans="1:40" ht="25.5" customHeight="1">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
-      <c r="N2" s="65"/>
-      <c r="O2" s="65"/>
-      <c r="P2" s="65"/>
-      <c r="Q2" s="65"/>
-      <c r="R2" s="65"/>
-      <c r="S2" s="65"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="58" t="s">
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="42"/>
+      <c r="R2" s="42"/>
+      <c r="S2" s="42"/>
+      <c r="T2" s="43"/>
+      <c r="U2" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="65"/>
-      <c r="W2" s="65"/>
-      <c r="X2" s="65"/>
-      <c r="Y2" s="65"/>
-      <c r="Z2" s="65"/>
-      <c r="AA2" s="65"/>
-      <c r="AB2" s="65"/>
-      <c r="AC2" s="65"/>
-      <c r="AD2" s="51"/>
-      <c r="AE2" s="66" t="s">
+      <c r="V2" s="42"/>
+      <c r="W2" s="42"/>
+      <c r="X2" s="42"/>
+      <c r="Y2" s="42"/>
+      <c r="Z2" s="42"/>
+      <c r="AA2" s="42"/>
+      <c r="AB2" s="42"/>
+      <c r="AC2" s="42"/>
+      <c r="AD2" s="43"/>
+      <c r="AE2" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="AF2" s="65"/>
-      <c r="AG2" s="65"/>
-      <c r="AH2" s="65"/>
-      <c r="AI2" s="65"/>
-      <c r="AJ2" s="65"/>
-      <c r="AK2" s="65"/>
-      <c r="AL2" s="51"/>
-      <c r="AM2" s="52" t="s">
+      <c r="AF2" s="42"/>
+      <c r="AG2" s="42"/>
+      <c r="AH2" s="42"/>
+      <c r="AI2" s="42"/>
+      <c r="AJ2" s="42"/>
+      <c r="AK2" s="42"/>
+      <c r="AL2" s="43"/>
+      <c r="AM2" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="AN2" s="53"/>
+      <c r="AN2" s="46"/>
     </row>
     <row r="3" spans="1:40" ht="25.5" customHeight="1">
-      <c r="A3" s="48"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="50" t="s">
+      <c r="A3" s="58"/>
+      <c r="B3" s="58"/>
+      <c r="C3" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="51"/>
-      <c r="E3" s="50" t="s">
+      <c r="D3" s="43"/>
+      <c r="E3" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="51"/>
-      <c r="G3" s="57" t="s">
+      <c r="F3" s="43"/>
+      <c r="G3" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="51"/>
-      <c r="I3" s="50" t="s">
+      <c r="H3" s="43"/>
+      <c r="I3" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="51"/>
-      <c r="K3" s="50" t="s">
+      <c r="J3" s="43"/>
+      <c r="K3" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="51"/>
-      <c r="M3" s="50" t="s">
+      <c r="L3" s="43"/>
+      <c r="M3" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="51"/>
-      <c r="O3" s="50" t="s">
+      <c r="N3" s="43"/>
+      <c r="O3" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="51"/>
-      <c r="Q3" s="50" t="s">
+      <c r="P3" s="43"/>
+      <c r="Q3" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="R3" s="51"/>
-      <c r="S3" s="50" t="s">
+      <c r="R3" s="43"/>
+      <c r="S3" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="T3" s="51"/>
-      <c r="U3" s="58" t="s">
+      <c r="T3" s="43"/>
+      <c r="U3" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="V3" s="51"/>
-      <c r="W3" s="59" t="s">
+      <c r="V3" s="43"/>
+      <c r="W3" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="X3" s="55"/>
-      <c r="Y3" s="60" t="s">
+      <c r="X3" s="48"/>
+      <c r="Y3" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="Z3" s="51"/>
-      <c r="AA3" s="60" t="s">
+      <c r="Z3" s="43"/>
+      <c r="AA3" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="AB3" s="51"/>
-      <c r="AC3" s="61" t="s">
+      <c r="AB3" s="43"/>
+      <c r="AC3" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="AD3" s="62"/>
-      <c r="AE3" s="63" t="s">
+      <c r="AD3" s="55"/>
+      <c r="AE3" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="AF3" s="62"/>
-      <c r="AG3" s="63" t="s">
+      <c r="AF3" s="55"/>
+      <c r="AG3" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="AH3" s="62"/>
-      <c r="AI3" s="56" t="s">
+      <c r="AH3" s="55"/>
+      <c r="AI3" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="AJ3" s="51"/>
-      <c r="AK3" s="56" t="s">
+      <c r="AJ3" s="43"/>
+      <c r="AK3" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="AL3" s="51"/>
-      <c r="AM3" s="54"/>
-      <c r="AN3" s="55"/>
+      <c r="AL3" s="43"/>
+      <c r="AM3" s="47"/>
+      <c r="AN3" s="48"/>
     </row>
     <row r="4" spans="1:40" ht="25.5" customHeight="1">
-      <c r="A4" s="49"/>
-      <c r="B4" s="49"/>
+      <c r="A4" s="59"/>
+      <c r="B4" s="59"/>
       <c r="C4" s="2" t="s">
         <v>20</v>
       </c>
@@ -1292,7 +1232,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -1338,7 +1278,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -1384,7 +1324,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -1430,7 +1370,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -1472,11 +1412,11 @@
       <c r="AN9" s="17"/>
     </row>
     <row r="10" spans="1:40" ht="12.75">
-      <c r="A10" s="47">
+      <c r="A10" s="57">
         <v>6</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
@@ -1518,9 +1458,9 @@
       <c r="AN10" s="17"/>
     </row>
     <row r="11" spans="1:40" ht="12.75">
-      <c r="A11" s="48"/>
+      <c r="A11" s="58"/>
       <c r="B11" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
@@ -1562,9 +1502,9 @@
       <c r="AN11" s="17"/>
     </row>
     <row r="12" spans="1:40" ht="12.75">
-      <c r="A12" s="48"/>
+      <c r="A12" s="58"/>
       <c r="B12" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
@@ -1606,9 +1546,9 @@
       <c r="AN12" s="17"/>
     </row>
     <row r="13" spans="1:40" ht="12.75">
-      <c r="A13" s="49"/>
+      <c r="A13" s="59"/>
       <c r="B13" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
@@ -1654,7 +1594,7 @@
         <v>7</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
@@ -1700,7 +1640,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="23"/>
       <c r="D15" s="23"/>
@@ -1746,7 +1686,7 @@
         <v>9</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="23"/>
       <c r="D16" s="23"/>
@@ -1792,7 +1732,7 @@
         <v>10</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" s="23"/>
       <c r="D17" s="23"/>
@@ -1838,7 +1778,7 @@
         <v>11</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
@@ -1884,7 +1824,7 @@
         <v>12</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
@@ -1930,7 +1870,7 @@
         <v>13</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
@@ -1976,7 +1916,7 @@
         <v>14</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
@@ -2022,7 +1962,7 @@
         <v>15</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
@@ -2068,7 +2008,7 @@
         <v>16</v>
       </c>
       <c r="B23" s="33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
@@ -2110,11 +2050,11 @@
       <c r="AN23" s="16"/>
     </row>
     <row r="24" spans="1:40" ht="12.75">
-      <c r="A24" s="47">
+      <c r="A24" s="57">
         <v>17</v>
       </c>
       <c r="B24" s="34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
@@ -2156,9 +2096,9 @@
       <c r="AN24" s="17"/>
     </row>
     <row r="25" spans="1:40" ht="12.75">
-      <c r="A25" s="48"/>
+      <c r="A25" s="58"/>
       <c r="B25" s="33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
@@ -2200,9 +2140,9 @@
       <c r="AN25" s="17"/>
     </row>
     <row r="26" spans="1:40" ht="12.75">
-      <c r="A26" s="48"/>
+      <c r="A26" s="58"/>
       <c r="B26" s="33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
@@ -2244,9 +2184,9 @@
       <c r="AN26" s="17"/>
     </row>
     <row r="27" spans="1:40" ht="12.75">
-      <c r="A27" s="49"/>
+      <c r="A27" s="59"/>
       <c r="B27" s="33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
@@ -2529,6 +2469,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="AG3:AH3"/>
+    <mergeCell ref="AI3:AJ3"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:T2"/>
     <mergeCell ref="U2:AD2"/>
     <mergeCell ref="AE2:AL2"/>
     <mergeCell ref="AM2:AN3"/>
@@ -2545,1260 +2495,9 @@
     <mergeCell ref="AA3:AB3"/>
     <mergeCell ref="AC3:AD3"/>
     <mergeCell ref="AE3:AF3"/>
-    <mergeCell ref="AG3:AH3"/>
-    <mergeCell ref="AI3:AJ3"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:T2"/>
   </mergeCells>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:AG13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="33" width="6.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:33">
-      <c r="A1" s="67" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" s="68" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="68" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="65"/>
-      <c r="S1" s="65"/>
-      <c r="T1" s="65"/>
-      <c r="U1" s="65"/>
-      <c r="V1" s="65"/>
-      <c r="W1" s="65"/>
-      <c r="X1" s="65"/>
-      <c r="Y1" s="51"/>
-      <c r="Z1" s="68" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA1" s="65"/>
-      <c r="AB1" s="65"/>
-      <c r="AC1" s="65"/>
-      <c r="AD1" s="65"/>
-      <c r="AE1" s="65"/>
-      <c r="AF1" s="65"/>
-      <c r="AG1" s="51"/>
-    </row>
-    <row r="2" spans="1:33">
-      <c r="A2" s="48"/>
-      <c r="B2" s="68" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="68" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="67" t="s">
-        <v>6</v>
-      </c>
-      <c r="P2" s="68" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q2" s="65"/>
-      <c r="R2" s="65"/>
-      <c r="S2" s="65"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="68" t="s">
-        <v>21</v>
-      </c>
-      <c r="V2" s="65"/>
-      <c r="W2" s="65"/>
-      <c r="X2" s="51"/>
-      <c r="Y2" s="67" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z2" s="68" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA2" s="65"/>
-      <c r="AB2" s="65"/>
-      <c r="AC2" s="51"/>
-      <c r="AD2" s="68" t="s">
-        <v>21</v>
-      </c>
-      <c r="AE2" s="65"/>
-      <c r="AF2" s="51"/>
-      <c r="AG2" s="67" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:33">
-      <c r="A3" s="49"/>
-      <c r="B3" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="41" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="41" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="K3" s="41" t="s">
-        <v>12</v>
-      </c>
-      <c r="L3" s="41" t="s">
-        <v>10</v>
-      </c>
-      <c r="M3" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="N3" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="O3" s="49"/>
-      <c r="P3" s="41" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q3" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="R3" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="S3" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="T3" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="U3" s="41" t="s">
-        <v>50</v>
-      </c>
-      <c r="V3" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="W3" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="X3" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y3" s="49"/>
-      <c r="Z3" s="41" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA3" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="AB3" s="41" t="s">
-        <v>19</v>
-      </c>
-      <c r="AC3" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="AD3" s="41" t="s">
-        <v>50</v>
-      </c>
-      <c r="AE3" s="41" t="s">
-        <v>19</v>
-      </c>
-      <c r="AF3" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="AG3" s="49"/>
-    </row>
-    <row r="4" spans="1:33">
-      <c r="A4" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="43">
-        <v>1168</v>
-      </c>
-      <c r="C4" s="43">
-        <v>111</v>
-      </c>
-      <c r="D4" s="43">
-        <v>112</v>
-      </c>
-      <c r="E4" s="43">
-        <v>29</v>
-      </c>
-      <c r="F4" s="43">
-        <v>10</v>
-      </c>
-      <c r="G4" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="41">
-        <v>1430</v>
-      </c>
-      <c r="I4" s="43">
-        <v>296</v>
-      </c>
-      <c r="J4" s="43">
-        <v>198</v>
-      </c>
-      <c r="K4" s="43">
-        <v>31</v>
-      </c>
-      <c r="L4" s="43">
-        <v>5</v>
-      </c>
-      <c r="M4" s="43">
-        <v>0</v>
-      </c>
-      <c r="N4" s="41">
-        <v>530</v>
-      </c>
-      <c r="O4" s="41">
-        <v>1960</v>
-      </c>
-      <c r="P4" s="44">
-        <v>651</v>
-      </c>
-      <c r="Q4" s="43">
-        <v>32</v>
-      </c>
-      <c r="R4" s="43">
-        <v>16</v>
-      </c>
-      <c r="S4" s="43">
-        <v>148</v>
-      </c>
-      <c r="T4" s="41">
-        <v>847</v>
-      </c>
-      <c r="U4" s="43">
-        <v>14</v>
-      </c>
-      <c r="V4" s="43">
-        <v>30</v>
-      </c>
-      <c r="W4" s="43">
-        <v>76</v>
-      </c>
-      <c r="X4" s="41">
-        <v>120</v>
-      </c>
-      <c r="Y4" s="41">
-        <v>970</v>
-      </c>
-      <c r="Z4" s="43">
-        <v>506</v>
-      </c>
-      <c r="AA4" s="43">
-        <v>5</v>
-      </c>
-      <c r="AB4" s="43">
-        <v>90</v>
-      </c>
-      <c r="AC4" s="41">
-        <v>601</v>
-      </c>
-      <c r="AD4" s="43">
-        <v>1</v>
-      </c>
-      <c r="AE4" s="43">
-        <v>33</v>
-      </c>
-      <c r="AF4" s="41">
-        <v>34</v>
-      </c>
-      <c r="AG4" s="41">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="5" spans="1:33">
-      <c r="A5" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5" s="43">
-        <v>55</v>
-      </c>
-      <c r="C5" s="43">
-        <v>18</v>
-      </c>
-      <c r="D5" s="43">
-        <v>8</v>
-      </c>
-      <c r="E5" s="43">
-        <v>13</v>
-      </c>
-      <c r="F5" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="41">
-        <v>94</v>
-      </c>
-      <c r="I5" s="43">
-        <v>12</v>
-      </c>
-      <c r="J5" s="43">
-        <v>19</v>
-      </c>
-      <c r="K5" s="43">
-        <v>0</v>
-      </c>
-      <c r="L5" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="M5" s="43">
-        <v>0</v>
-      </c>
-      <c r="N5" s="41">
-        <v>31</v>
-      </c>
-      <c r="O5" s="41">
-        <v>125</v>
-      </c>
-      <c r="P5" s="43">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="43">
-        <v>0</v>
-      </c>
-      <c r="R5" s="43">
-        <v>0</v>
-      </c>
-      <c r="S5" s="43">
-        <v>0</v>
-      </c>
-      <c r="T5" s="41">
-        <v>0</v>
-      </c>
-      <c r="U5" s="43">
-        <v>0</v>
-      </c>
-      <c r="V5" s="43">
-        <v>0</v>
-      </c>
-      <c r="W5" s="43">
-        <v>0</v>
-      </c>
-      <c r="X5" s="41">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="41">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA5" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB5" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC5" s="41">
-        <v>0</v>
-      </c>
-      <c r="AD5" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE5" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AF5" s="41">
-        <v>0</v>
-      </c>
-      <c r="AG5" s="41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:33">
-      <c r="A6" s="42" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="43">
-        <v>208</v>
-      </c>
-      <c r="C6" s="43">
-        <v>12</v>
-      </c>
-      <c r="D6" s="43">
-        <v>61</v>
-      </c>
-      <c r="E6" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="43">
-        <v>15</v>
-      </c>
-      <c r="G6" s="43">
-        <v>9</v>
-      </c>
-      <c r="H6" s="41">
-        <v>305</v>
-      </c>
-      <c r="I6" s="43">
-        <v>0</v>
-      </c>
-      <c r="J6" s="43">
-        <v>1</v>
-      </c>
-      <c r="K6" s="43">
-        <v>0</v>
-      </c>
-      <c r="L6" s="43">
-        <v>1</v>
-      </c>
-      <c r="M6" s="43">
-        <v>13</v>
-      </c>
-      <c r="N6" s="41">
-        <v>15</v>
-      </c>
-      <c r="O6" s="41">
-        <v>320</v>
-      </c>
-      <c r="P6" s="44">
-        <v>120</v>
-      </c>
-      <c r="Q6" s="43">
-        <v>12</v>
-      </c>
-      <c r="R6" s="43">
-        <v>0</v>
-      </c>
-      <c r="S6" s="43">
-        <v>0</v>
-      </c>
-      <c r="T6" s="41">
-        <v>132</v>
-      </c>
-      <c r="U6" s="43">
-        <v>0</v>
-      </c>
-      <c r="V6" s="43">
-        <v>0</v>
-      </c>
-      <c r="W6" s="43">
-        <v>0</v>
-      </c>
-      <c r="X6" s="41">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="41">
-        <v>139</v>
-      </c>
-      <c r="Z6" s="43">
-        <v>28</v>
-      </c>
-      <c r="AA6" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB6" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC6" s="41">
-        <v>28</v>
-      </c>
-      <c r="AD6" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE6" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AF6" s="41">
-        <v>0</v>
-      </c>
-      <c r="AG6" s="41">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:33">
-      <c r="A7" s="42" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" s="43">
-        <v>13</v>
-      </c>
-      <c r="C7" s="43">
-        <v>172</v>
-      </c>
-      <c r="D7" s="43">
-        <v>36</v>
-      </c>
-      <c r="E7" s="43">
-        <v>39</v>
-      </c>
-      <c r="F7" s="43">
-        <v>5</v>
-      </c>
-      <c r="G7" s="43">
-        <v>13</v>
-      </c>
-      <c r="H7" s="41">
-        <v>278</v>
-      </c>
-      <c r="I7" s="43">
-        <v>18</v>
-      </c>
-      <c r="J7" s="43">
-        <v>0</v>
-      </c>
-      <c r="K7" s="43">
-        <v>1</v>
-      </c>
-      <c r="L7" s="43">
-        <v>0</v>
-      </c>
-      <c r="M7" s="43">
-        <v>15</v>
-      </c>
-      <c r="N7" s="41">
-        <v>34</v>
-      </c>
-      <c r="O7" s="41">
-        <v>312</v>
-      </c>
-      <c r="P7" s="43">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="43">
-        <v>0</v>
-      </c>
-      <c r="R7" s="43">
-        <v>15</v>
-      </c>
-      <c r="S7" s="43">
-        <v>13</v>
-      </c>
-      <c r="T7" s="41">
-        <v>28</v>
-      </c>
-      <c r="U7" s="43">
-        <v>0</v>
-      </c>
-      <c r="V7" s="43">
-        <v>0</v>
-      </c>
-      <c r="W7" s="43">
-        <v>0</v>
-      </c>
-      <c r="X7" s="41">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="41">
-        <v>38</v>
-      </c>
-      <c r="Z7" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA7" s="43">
-        <v>15</v>
-      </c>
-      <c r="AB7" s="43">
-        <v>5</v>
-      </c>
-      <c r="AC7" s="41">
-        <v>20</v>
-      </c>
-      <c r="AD7" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE7" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AF7" s="41">
-        <v>0</v>
-      </c>
-      <c r="AG7" s="41">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:33">
-      <c r="A8" s="42" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" s="43">
-        <v>3</v>
-      </c>
-      <c r="C8" s="43">
-        <v>0</v>
-      </c>
-      <c r="D8" s="43">
-        <v>15</v>
-      </c>
-      <c r="E8" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="43">
-        <v>2</v>
-      </c>
-      <c r="G8" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="41">
-        <v>20</v>
-      </c>
-      <c r="I8" s="43">
-        <v>0</v>
-      </c>
-      <c r="J8" s="43">
-        <v>3</v>
-      </c>
-      <c r="K8" s="43">
-        <v>0</v>
-      </c>
-      <c r="L8" s="43">
-        <v>3</v>
-      </c>
-      <c r="M8" s="43">
-        <v>0</v>
-      </c>
-      <c r="N8" s="41">
-        <v>6</v>
-      </c>
-      <c r="O8" s="41">
-        <v>26</v>
-      </c>
-      <c r="P8" s="44">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="43">
-        <v>0</v>
-      </c>
-      <c r="R8" s="43">
-        <v>2</v>
-      </c>
-      <c r="S8" s="43">
-        <v>0</v>
-      </c>
-      <c r="T8" s="41">
-        <v>2</v>
-      </c>
-      <c r="U8" s="43">
-        <v>0</v>
-      </c>
-      <c r="V8" s="43">
-        <v>0</v>
-      </c>
-      <c r="W8" s="43">
-        <v>0</v>
-      </c>
-      <c r="X8" s="41">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="41">
-        <v>7</v>
-      </c>
-      <c r="Z8" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA8" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB8" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC8" s="41">
-        <v>0</v>
-      </c>
-      <c r="AD8" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE8" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AF8" s="41">
-        <v>0</v>
-      </c>
-      <c r="AG8" s="41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:33">
-      <c r="A9" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="43">
-        <v>0</v>
-      </c>
-      <c r="C9" s="43">
-        <v>0</v>
-      </c>
-      <c r="D9" s="43">
-        <v>0</v>
-      </c>
-      <c r="E9" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="43">
-        <v>0</v>
-      </c>
-      <c r="G9" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="41">
-        <v>0</v>
-      </c>
-      <c r="I9" s="43">
-        <v>0</v>
-      </c>
-      <c r="J9" s="43">
-        <v>0</v>
-      </c>
-      <c r="K9" s="43">
-        <v>0</v>
-      </c>
-      <c r="L9" s="43">
-        <v>0</v>
-      </c>
-      <c r="M9" s="43">
-        <v>0</v>
-      </c>
-      <c r="N9" s="41">
-        <v>0</v>
-      </c>
-      <c r="O9" s="41">
-        <v>0</v>
-      </c>
-      <c r="P9" s="43">
-        <v>2</v>
-      </c>
-      <c r="Q9" s="43">
-        <v>0</v>
-      </c>
-      <c r="R9" s="43">
-        <v>0</v>
-      </c>
-      <c r="S9" s="43">
-        <v>2</v>
-      </c>
-      <c r="T9" s="41">
-        <v>4</v>
-      </c>
-      <c r="U9" s="43">
-        <v>0</v>
-      </c>
-      <c r="V9" s="43">
-        <v>0</v>
-      </c>
-      <c r="W9" s="43">
-        <v>0</v>
-      </c>
-      <c r="X9" s="41">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="41">
-        <v>5</v>
-      </c>
-      <c r="Z9" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA9" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB9" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC9" s="41">
-        <v>0</v>
-      </c>
-      <c r="AD9" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE9" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AF9" s="41">
-        <v>0</v>
-      </c>
-      <c r="AG9" s="41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:33">
-      <c r="A10" s="42" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10" s="43">
-        <v>4</v>
-      </c>
-      <c r="C10" s="43">
-        <v>0</v>
-      </c>
-      <c r="D10" s="43">
-        <v>6</v>
-      </c>
-      <c r="E10" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="43">
-        <v>2</v>
-      </c>
-      <c r="G10" s="43">
-        <v>21</v>
-      </c>
-      <c r="H10" s="41">
-        <v>33</v>
-      </c>
-      <c r="I10" s="43">
-        <v>0</v>
-      </c>
-      <c r="J10" s="43">
-        <v>0</v>
-      </c>
-      <c r="K10" s="43">
-        <v>0</v>
-      </c>
-      <c r="L10" s="43">
-        <v>0</v>
-      </c>
-      <c r="M10" s="43">
-        <v>1</v>
-      </c>
-      <c r="N10" s="41">
-        <v>1</v>
-      </c>
-      <c r="O10" s="41">
-        <v>34</v>
-      </c>
-      <c r="P10" s="43">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="43">
-        <v>0</v>
-      </c>
-      <c r="R10" s="43">
-        <v>0</v>
-      </c>
-      <c r="S10" s="43">
-        <v>0</v>
-      </c>
-      <c r="T10" s="41">
-        <v>0</v>
-      </c>
-      <c r="U10" s="43">
-        <v>0</v>
-      </c>
-      <c r="V10" s="43">
-        <v>0</v>
-      </c>
-      <c r="W10" s="43">
-        <v>0</v>
-      </c>
-      <c r="X10" s="41">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="41">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA10" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB10" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC10" s="41">
-        <v>0</v>
-      </c>
-      <c r="AD10" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE10" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AF10" s="41">
-        <v>0</v>
-      </c>
-      <c r="AG10" s="41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:33">
-      <c r="A11" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" s="43">
-        <v>4</v>
-      </c>
-      <c r="C11" s="43">
-        <v>2</v>
-      </c>
-      <c r="D11" s="43">
-        <v>24</v>
-      </c>
-      <c r="E11" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="43">
-        <v>0</v>
-      </c>
-      <c r="G11" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" s="41">
-        <v>30</v>
-      </c>
-      <c r="I11" s="43">
-        <v>0</v>
-      </c>
-      <c r="J11" s="43">
-        <v>11</v>
-      </c>
-      <c r="K11" s="43">
-        <v>0</v>
-      </c>
-      <c r="L11" s="43">
-        <v>0</v>
-      </c>
-      <c r="M11" s="43">
-        <v>9</v>
-      </c>
-      <c r="N11" s="41">
-        <v>20</v>
-      </c>
-      <c r="O11" s="41">
-        <v>50</v>
-      </c>
-      <c r="P11" s="43">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="43">
-        <v>0</v>
-      </c>
-      <c r="R11" s="43">
-        <v>0</v>
-      </c>
-      <c r="S11" s="43">
-        <v>0</v>
-      </c>
-      <c r="T11" s="41">
-        <v>0</v>
-      </c>
-      <c r="U11" s="43">
-        <v>0</v>
-      </c>
-      <c r="V11" s="43">
-        <v>0</v>
-      </c>
-      <c r="W11" s="43">
-        <v>0</v>
-      </c>
-      <c r="X11" s="41">
-        <v>0</v>
-      </c>
-      <c r="Y11" s="41">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA11" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB11" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC11" s="41">
-        <v>0</v>
-      </c>
-      <c r="AD11" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE11" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AF11" s="41">
-        <v>0</v>
-      </c>
-      <c r="AG11" s="41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:33">
-      <c r="A12" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="B12" s="43">
-        <v>14</v>
-      </c>
-      <c r="C12" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12" s="41">
-        <v>14</v>
-      </c>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43"/>
-      <c r="K12" s="43"/>
-      <c r="L12" s="43"/>
-      <c r="M12" s="43"/>
-      <c r="N12" s="41">
-        <v>0</v>
-      </c>
-      <c r="O12" s="41">
-        <v>14</v>
-      </c>
-      <c r="P12" s="44">
-        <v>89</v>
-      </c>
-      <c r="Q12" s="43">
-        <v>147</v>
-      </c>
-      <c r="R12" s="43">
-        <v>0</v>
-      </c>
-      <c r="S12" s="43">
-        <v>153</v>
-      </c>
-      <c r="T12" s="41">
-        <v>389</v>
-      </c>
-      <c r="U12" s="43">
-        <v>12</v>
-      </c>
-      <c r="V12" s="43">
-        <v>46</v>
-      </c>
-      <c r="W12" s="43">
-        <v>0</v>
-      </c>
-      <c r="X12" s="41">
-        <v>58</v>
-      </c>
-      <c r="Y12" s="41">
-        <v>416</v>
-      </c>
-      <c r="Z12" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA12" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB12" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC12" s="41">
-        <v>0</v>
-      </c>
-      <c r="AD12" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE12" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AF12" s="41">
-        <v>0</v>
-      </c>
-      <c r="AG12" s="41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:33">
-      <c r="A13" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="45">
-        <f t="shared" ref="B13:E13" si="0">SUM(B4:B12)</f>
-        <v>1469</v>
-      </c>
-      <c r="C13" s="45">
-        <f t="shared" si="0"/>
-        <v>315</v>
-      </c>
-      <c r="D13" s="45">
-        <f t="shared" si="0"/>
-        <v>262</v>
-      </c>
-      <c r="E13" s="45">
-        <f t="shared" si="0"/>
-        <v>81</v>
-      </c>
-      <c r="F13" s="45">
-        <v>34</v>
-      </c>
-      <c r="G13" s="45">
-        <v>43</v>
-      </c>
-      <c r="H13" s="45">
-        <v>2204</v>
-      </c>
-      <c r="I13" s="45">
-        <v>326</v>
-      </c>
-      <c r="J13" s="45">
-        <v>232</v>
-      </c>
-      <c r="K13" s="45">
-        <v>32</v>
-      </c>
-      <c r="L13" s="45">
-        <v>9</v>
-      </c>
-      <c r="M13" s="45">
-        <v>38</v>
-      </c>
-      <c r="N13" s="45">
-        <v>637</v>
-      </c>
-      <c r="O13" s="45">
-        <v>2841</v>
-      </c>
-      <c r="P13" s="46">
-        <f t="shared" ref="P13:Y13" si="1">SUM(P4:P12)</f>
-        <v>862</v>
-      </c>
-      <c r="Q13" s="46">
-        <f t="shared" si="1"/>
-        <v>191</v>
-      </c>
-      <c r="R13" s="46">
-        <f t="shared" si="1"/>
-        <v>33</v>
-      </c>
-      <c r="S13" s="46">
-        <f t="shared" si="1"/>
-        <v>316</v>
-      </c>
-      <c r="T13" s="46">
-        <f t="shared" si="1"/>
-        <v>1402</v>
-      </c>
-      <c r="U13" s="46">
-        <f t="shared" si="1"/>
-        <v>26</v>
-      </c>
-      <c r="V13" s="46">
-        <f t="shared" si="1"/>
-        <v>76</v>
-      </c>
-      <c r="W13" s="46">
-        <f t="shared" si="1"/>
-        <v>76</v>
-      </c>
-      <c r="X13" s="46">
-        <f t="shared" si="1"/>
-        <v>178</v>
-      </c>
-      <c r="Y13" s="46">
-        <f t="shared" si="1"/>
-        <v>1575</v>
-      </c>
-      <c r="Z13" s="45">
-        <v>534</v>
-      </c>
-      <c r="AA13" s="45">
-        <v>20</v>
-      </c>
-      <c r="AB13" s="45">
-        <v>95</v>
-      </c>
-      <c r="AC13" s="45">
-        <v>649</v>
-      </c>
-      <c r="AD13" s="45">
-        <v>1</v>
-      </c>
-      <c r="AE13" s="45">
-        <v>33</v>
-      </c>
-      <c r="AF13" s="45">
-        <v>34</v>
-      </c>
-      <c r="AG13" s="45">
-        <v>683</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="AG2:AG3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:O1"/>
-    <mergeCell ref="P1:Y1"/>
-    <mergeCell ref="Z1:AG1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="P2:T2"/>
-    <mergeCell ref="U2:X2"/>
-    <mergeCell ref="Y2:Y3"/>
-    <mergeCell ref="Z2:AC2"/>
-    <mergeCell ref="AD2:AF2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>